<commit_message>
Finally figured out how to read in a table!!!!
</commit_message>
<xml_diff>
--- a/toy_dataset.xlsx
+++ b/toy_dataset.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17347\Documents\GitHub\D2P-Spring-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{269BA9F4-ACCB-4353-9237-66F7AF23186F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A00EDB-ED26-46D9-9A73-03D91E9679BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-26700" yWindow="1725" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="toy_dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="Toydata">Sheet1!$A$1:$L$9</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,43 +37,43 @@
     <t>Item</t>
   </si>
   <si>
-    <t>Group _1_1</t>
-  </si>
-  <si>
-    <t>Group_1_2</t>
-  </si>
-  <si>
-    <t>Group_2_1</t>
-  </si>
-  <si>
-    <t>Group_2_2</t>
-  </si>
-  <si>
-    <t>Group_2_3</t>
-  </si>
-  <si>
-    <t>Group_2_4</t>
-  </si>
-  <si>
-    <t>Group_3_1</t>
-  </si>
-  <si>
-    <t>Group_3_2</t>
-  </si>
-  <si>
-    <t>Group_3_3</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
-    <t>Group_1_3</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -73,6 +85,104 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,83 +196,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,29 +205,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,12 +219,165 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
@@ -222,160 +387,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -385,6 +397,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -415,17 +457,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -447,45 +498,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -497,94 +509,94 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -895,11 +907,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F51AD65-77D1-429B-81E2-01A3156949B9}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,37 +927,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleaned up some things
</commit_message>
<xml_diff>
--- a/toy_dataset.xlsx
+++ b/toy_dataset.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17347\Documents\GitHub\D2P-Spring-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A00EDB-ED26-46D9-9A73-03D91E9679BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F76AF1-104B-4875-90BB-8313362ED5B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26700" yWindow="1725" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="5175" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Toydata">Sheet1!$A$1:$L$9</definedName>
+    <definedName name="FeatToyData">Sheet1!$A$16:$K$24</definedName>
+    <definedName name="NegToyData">Sheet1!$A$1:$K$3</definedName>
+    <definedName name="PosToyData">Sheet1!$A$7:$K$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,42 +34,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
-    <t>Item</t>
+    <t>Sample</t>
   </si>
   <si>
-    <t>Result</t>
+    <t>Feat1</t>
   </si>
   <si>
-    <t>A</t>
+    <t>Feat2</t>
   </si>
   <si>
-    <t>B</t>
+    <t>Feat3</t>
   </si>
   <si>
-    <t>C</t>
+    <t>Feat5</t>
   </si>
   <si>
-    <t>D</t>
+    <t>Feat6</t>
   </si>
   <si>
-    <t>E</t>
+    <t>Feat7</t>
   </si>
   <si>
-    <t>F</t>
+    <t>Feat8</t>
   </si>
   <si>
-    <t>G</t>
+    <t>Feat9</t>
   </si>
   <si>
-    <t>H</t>
+    <t>Feat10</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
+    <t>Feat4</t>
   </si>
 </sst>
 </file>
@@ -908,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F51AD65-77D1-429B-81E2-01A3156949B9}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,45 +921,42 @@
     <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -974,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -983,30 +979,27 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1015,253 +1008,582 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="G7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="H7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="J16" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>